<commit_message>
Clean up + connecting to database
</commit_message>
<xml_diff>
--- a/media/shp/murale_ursynow.xlsx
+++ b/media/shp/murale_ursynow.xlsx
@@ -1,19 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sebas\OneDrive\Pulpit\Projekty\murals\data\interim\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\Projects\geo-murals\media\shp\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC2C8F7-6C3B-4ECB-BCD8-5DEF105BB7D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9276"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Arkusz1!$A$1:$D$1</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -374,7 +378,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -686,22 +690,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30:D30"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="4" max="4" width="23.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>10</v>
       </c>
@@ -715,7 +718,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -729,7 +732,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>41</v>
       </c>
@@ -743,7 +746,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>42</v>
       </c>
@@ -757,7 +760,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>43</v>
       </c>
@@ -771,7 +774,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -785,7 +788,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>37</v>
       </c>
@@ -799,7 +802,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>38</v>
       </c>
@@ -813,7 +816,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>39</v>
       </c>
@@ -827,7 +830,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>44</v>
       </c>
@@ -841,7 +844,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -855,7 +858,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -869,7 +872,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>54</v>
       </c>
@@ -883,7 +886,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -897,7 +900,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
@@ -911,7 +914,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -925,7 +928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>56</v>
       </c>
@@ -939,7 +942,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>47</v>
       </c>
@@ -953,7 +956,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -967,7 +970,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>48</v>
       </c>
@@ -981,7 +984,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -995,7 +998,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>49</v>
       </c>
@@ -1009,7 +1012,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>58</v>
       </c>
@@ -1023,7 +1026,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1037,7 +1040,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1051,7 +1054,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>40</v>
       </c>
@@ -1065,7 +1068,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -1079,7 +1082,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>52</v>
       </c>
@@ -1093,7 +1096,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>53</v>
       </c>
@@ -1108,6 +1111,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>